<commit_message>
added expection module and two negative tests
</commit_message>
<xml_diff>
--- a/text_docs/Test_Plan_bank.xlsx
+++ b/text_docs/Test_Plan_bank.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26529"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="11_556E44F040EC6D42B43B847BF7AA6B5224D9E9BF" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9A27384A-9388-4C23-BC84-2AE0675D563A}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="59">
   <si>
     <t>Project Name</t>
   </si>
@@ -67,9 +68,6 @@
   </si>
   <si>
     <t>Comments</t>
-  </si>
-  <si>
-    <t>TC-001</t>
   </si>
   <si>
     <t>1.Click onRegister button
@@ -115,7 +113,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
+        <rFont val="Arial"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -125,7 +123,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="Arial"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -288,7 +286,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
+        <rFont val="Arial"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -298,7 +296,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="Arial"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -312,23 +310,29 @@
     <t xml:space="preserve">Fail and get message that usrname is already in use
 </t>
   </si>
+  <si>
+    <t>tc-001</t>
+  </si>
+  <si>
+    <t>Pass</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -336,7 +340,7 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -367,7 +371,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -382,21 +386,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -673,22 +680,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H54" sqref="H54"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="42.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.21875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="69.88671875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="64.109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="42.08203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.58203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.25" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="69.9140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="64.08203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.58203125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="29" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -758,247 +765,253 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:8" s="8" customFormat="1" ht="144" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" s="6" customFormat="1" ht="140" x14ac:dyDescent="0.3">
       <c r="A8" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B8" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="C8" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="F8" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="G8" s="9" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="140" x14ac:dyDescent="0.3">
+      <c r="A9" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="G9" s="10" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="140" x14ac:dyDescent="0.3">
+      <c r="A10" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="F10" s="7" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="70" x14ac:dyDescent="0.3">
+      <c r="A11" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="F11" s="7" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="42" x14ac:dyDescent="0.3">
+      <c r="A12" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E12" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="F12" s="7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="42" x14ac:dyDescent="0.3">
+      <c r="A13" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="F13" s="7" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="56" x14ac:dyDescent="0.3">
+      <c r="A14" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="C8" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="D8" s="8" t="s">
+      <c r="B14" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E14" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="F14" s="5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="70" x14ac:dyDescent="0.3">
+      <c r="A15" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E15" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="F15" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="H15" s="5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="56" x14ac:dyDescent="0.3">
+      <c r="A16" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E16" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="F16" s="5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="56" x14ac:dyDescent="0.3">
+      <c r="A17" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E17" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="F17" s="5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="70" x14ac:dyDescent="0.3">
+      <c r="A18" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="D18" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E18" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="F18" s="8" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="42" x14ac:dyDescent="0.3">
+      <c r="A19" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="D19" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="E8" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="F8" s="7" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="158.4" x14ac:dyDescent="0.3">
-      <c r="A9" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="B9" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="C9" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="D9" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="E9" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="F9" s="7" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" ht="144" x14ac:dyDescent="0.3">
-      <c r="A10" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="B10" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="C10" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="D10" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="E10" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="F10" s="7" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" ht="72" x14ac:dyDescent="0.3">
-      <c r="A11" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="B11" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="C11" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="D11" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="E11" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="F11" s="7" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A12" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="B12" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="C12" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="D12" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="E12" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="F12" s="7" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A13" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="B13" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="C13" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="D13" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="E13" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="F13" s="7" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A14" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="B14" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="C14" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="D14" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="E14" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="F14" s="5" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" ht="72" x14ac:dyDescent="0.3">
-      <c r="A15" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="B15" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="C15" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="D15" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="E15" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="F15" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="H15" s="5" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A16" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="B16" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="C16" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="D16" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="E16" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="F16" s="5" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A17" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="B17" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="C17" s="8" t="s">
+      <c r="E19" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="D17" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="E17" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="F17" s="5" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" ht="72" x14ac:dyDescent="0.3">
-      <c r="A18" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="B18" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="C18" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="D18" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="E18" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="F18" s="9" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A19" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="B19" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="C19" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="D19" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="E19" s="7" t="s">
+      <c r="F19" s="8" t="s">
         <v>50</v>
-      </c>
-      <c r="F19" s="9" t="s">
-        <v>51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
upgraded dropdown selector function whcih now gets index value to
</commit_message>
<xml_diff>
--- a/text_docs/Test_Plan_bank.xlsx
+++ b/text_docs/Test_Plan_bank.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26529"/>
-  <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="4" documentId="11_556E44F040EC6D42B43B847BF7AA6B5224D9E9BF" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9A27384A-9388-4C23-BC84-2AE0675D563A}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="19416" windowHeight="10296"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -20,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="57">
   <si>
     <t>Project Name</t>
   </si>
@@ -113,7 +112,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -123,7 +122,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Arial"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -222,11 +221,6 @@
     <t>Must see main page with no account details</t>
   </si>
   <si>
-    <t>1.At Amounts overview must be acount from where money was sent
-2.there must be Acount details
-3.Balance must be updated corectly depending on transaction amounts</t>
-  </si>
-  <si>
     <t xml:space="preserve"> 1.At Amounts overview must be acount from where money was sent
 2.there must be Acount details
 3.Balance must be updated corectly depending on transaction amounts</t>
@@ -268,9 +262,6 @@
   </si>
   <si>
     <t>TC-011</t>
-  </si>
-  <si>
-    <t>TC-012</t>
   </si>
   <si>
     <r>
@@ -286,7 +277,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -296,7 +287,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Arial"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -320,19 +311,19 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -340,7 +331,7 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -403,7 +394,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -680,22 +671,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView tabSelected="1" topLeftCell="B16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="42.08203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.58203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.25" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="69.9140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="64.08203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.58203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="42.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.21875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="69.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="64.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.5546875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="29" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -765,7 +756,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:8" s="6" customFormat="1" ht="140" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" s="6" customFormat="1" ht="144" x14ac:dyDescent="0.3">
       <c r="A8" s="6" t="s">
         <v>29</v>
       </c>
@@ -773,7 +764,7 @@
         <v>30</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D8" s="6" t="s">
         <v>18</v>
@@ -785,10 +776,10 @@
         <v>17</v>
       </c>
       <c r="G8" s="9" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="140" x14ac:dyDescent="0.3">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="144" x14ac:dyDescent="0.3">
       <c r="A9" s="6" t="s">
         <v>29</v>
       </c>
@@ -808,10 +799,10 @@
         <v>27</v>
       </c>
       <c r="G9" s="10" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" ht="140" x14ac:dyDescent="0.3">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="144" x14ac:dyDescent="0.3">
       <c r="A10" s="6" t="s">
         <v>29</v>
       </c>
@@ -825,13 +816,13 @@
         <v>19</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" ht="70" x14ac:dyDescent="0.3">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="72" x14ac:dyDescent="0.3">
       <c r="A11" s="6" t="s">
         <v>29</v>
       </c>
@@ -851,7 +842,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="42" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A12" s="6" t="s">
         <v>29</v>
       </c>
@@ -859,7 +850,7 @@
         <v>30</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D12" s="6" t="s">
         <v>19</v>
@@ -871,7 +862,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="42" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A13" s="6" t="s">
         <v>29</v>
       </c>
@@ -891,7 +882,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="56" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A14" s="6" t="s">
         <v>31</v>
       </c>
@@ -899,7 +890,7 @@
         <v>32</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D14" s="6" t="s">
         <v>18</v>
@@ -911,7 +902,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="70" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" ht="72" x14ac:dyDescent="0.3">
       <c r="A15" s="6" t="s">
         <v>31</v>
       </c>
@@ -934,7 +925,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="56" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A16" s="6" t="s">
         <v>31</v>
       </c>
@@ -942,7 +933,7 @@
         <v>32</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D16" s="6" t="s">
         <v>18</v>
@@ -951,30 +942,18 @@
         <v>39</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" ht="56" x14ac:dyDescent="0.3">
-      <c r="A17" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="B17" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="C17" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="D17" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="E17" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="F17" s="5" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="70" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17" s="6"/>
+      <c r="B17" s="7"/>
+      <c r="C17" s="6"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="7"/>
+      <c r="F17" s="5"/>
+    </row>
+    <row r="18" spans="1:6" ht="72" x14ac:dyDescent="0.3">
       <c r="A18" s="6" t="s">
         <v>31</v>
       </c>
@@ -982,19 +961,19 @@
         <v>32</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="D18" s="6" t="s">
         <v>18</v>
       </c>
       <c r="E18" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="F18" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="F18" s="8" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" ht="42" x14ac:dyDescent="0.3">
+    </row>
+    <row r="19" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A19" s="6" t="s">
         <v>31</v>
       </c>
@@ -1002,16 +981,16 @@
         <v>32</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D19" s="6" t="s">
         <v>19</v>
       </c>
       <c r="E19" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="F19" s="8" t="s">
         <v>49</v>
-      </c>
-      <c r="F19" s="8" t="s">
-        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added transaction finding by amount test
</commit_message>
<xml_diff>
--- a/text_docs/Test_Plan_bank.xlsx
+++ b/text_docs/Test_Plan_bank.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="54">
   <si>
     <t>Project Name</t>
   </si>
@@ -204,12 +204,6 @@
 with various amounts of money</t>
   </si>
   <si>
-    <t xml:space="preserve">1.At account servicies click Accounts overview
-2.Go to account from where money was transsfered
-3.Check balance
-</t>
-  </si>
-  <si>
     <t>TC-008</t>
   </si>
   <si>
@@ -219,11 +213,6 @@
   </si>
   <si>
     <t>Must see main page with no account details</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 1.At Amounts overview must be acount from where money was sent
-2.there must be Acount details
-3.Balance must be updated corectly depending on transaction amounts</t>
   </si>
   <si>
     <t>TC-009</t>
@@ -259,9 +248,6 @@
   </si>
   <si>
     <t>TC-07</t>
-  </si>
-  <si>
-    <t>TC-011</t>
   </si>
   <si>
     <r>
@@ -674,7 +660,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B16" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B14" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
@@ -764,7 +750,7 @@
         <v>30</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D8" s="6" t="s">
         <v>18</v>
@@ -776,7 +762,7 @@
         <v>17</v>
       </c>
       <c r="G8" s="9" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="144" x14ac:dyDescent="0.3">
@@ -799,7 +785,7 @@
         <v>27</v>
       </c>
       <c r="G9" s="10" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="144" x14ac:dyDescent="0.3">
@@ -816,10 +802,10 @@
         <v>19</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="72" x14ac:dyDescent="0.3">
@@ -850,7 +836,7 @@
         <v>30</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D12" s="6" t="s">
         <v>19</v>
@@ -876,10 +862,10 @@
         <v>18</v>
       </c>
       <c r="E13" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="F13" s="7" t="s">
         <v>41</v>
-      </c>
-      <c r="F13" s="7" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
@@ -890,7 +876,7 @@
         <v>32</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D14" s="6" t="s">
         <v>18</v>
@@ -910,7 +896,7 @@
         <v>32</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D15" s="6" t="s">
         <v>18</v>
@@ -925,25 +911,13 @@
         <v>38</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A16" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="B16" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="C16" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="D16" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="E16" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="F16" s="5" t="s">
-        <v>43</v>
-      </c>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A16" s="6"/>
+      <c r="B16" s="7"/>
+      <c r="C16" s="6"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="7"/>
+      <c r="F16" s="5"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="6"/>
@@ -961,16 +935,16 @@
         <v>32</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="D18" s="6" t="s">
         <v>18</v>
       </c>
       <c r="E18" s="7" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="F18" s="8" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
@@ -981,16 +955,16 @@
         <v>32</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="D19" s="6" t="s">
         <v>19</v>
       </c>
       <c r="E19" s="7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="F19" s="8" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>